<commit_message>
ROBE-218 refactoring and xlsx import test fix
</commit_message>
<xml_diff>
--- a/robe-convert/src/test/resources/sample.xlsx
+++ b/robe-convert/src/test/resources/sample.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="19020" tabRatio="500"/>
+    <workbookView xWindow="-23140" yWindow="-20160" windowWidth="14940" windowHeight="12920"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="SamplePojo" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,21 +19,51 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
-  <si>
-    <t>Guner Kaan ALKIM</t>
-  </si>
-  <si>
-    <t>Computer Engineer</t>
-  </si>
-  <si>
-    <t>12.12.2312</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+  <si>
+    <t>Seray</t>
+  </si>
+  <si>
+    <t>Uzgur</t>
+  </si>
+  <si>
+    <t>01.01.2014</t>
+  </si>
+  <si>
+    <t>Kaan</t>
+  </si>
+  <si>
+    <t>Alkim</t>
+  </si>
+  <si>
+    <t>02.01.2014</t>
   </si>
   <si>
     <t>Sinan</t>
   </si>
   <si>
-    <t>15.12.2312</t>
+    <t>Selimogli</t>
+  </si>
+  <si>
+    <t>03.01.2014</t>
+  </si>
+  <si>
+    <t>Kamil</t>
+  </si>
+  <si>
+    <t>Bukum</t>
+  </si>
+  <si>
+    <t>04.01.2014</t>
+  </si>
+  <si>
+    <t>Hasan</t>
+  </si>
+  <si>
+    <t>Mumin</t>
+  </si>
+  <si>
+    <t>05.01.2014</t>
   </si>
 </sst>
 </file>
@@ -42,27 +72,20 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <sz val="10"/>
+      <name val="Arial"/>
     </font>
     <font>
       <u/>
-      <sz val="12"/>
+      <sz val="10"/>
       <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <name val="Arial"/>
     </font>
     <font>
       <u/>
-      <sz val="12"/>
+      <sz val="10"/>
       <color theme="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="2">
@@ -101,6 +124,74 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00DD0806"/>
+      <rgbColor rgb="001FB714"/>
+      <rgbColor rgb="000000D4"/>
+      <rgbColor rgb="00FCF305"/>
+      <rgbColor rgb="00F20884"/>
+      <rgbColor rgb="0000ABEA"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00DD0806"/>
+      <rgbColor rgb="001FB714"/>
+      <rgbColor rgb="000000D4"/>
+      <rgbColor rgb="00FCF305"/>
+      <rgbColor rgb="00F20884"/>
+      <rgbColor rgb="0000ABEA"/>
+      <rgbColor rgb="00900000"/>
+      <rgbColor rgb="00006411"/>
+      <rgbColor rgb="00000090"/>
+      <rgbColor rgb="0090713A"/>
+      <rgbColor rgb="004600A5"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -426,13 +517,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="12" customWidth="1"/>
+    <col min="2" max="2" width="10" customWidth="1"/>
+    <col min="7" max="7" width="9.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1">
@@ -445,13 +541,13 @@
         <v>1</v>
       </c>
       <c r="D1">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="E1">
-        <v>2</v>
+        <v>111</v>
       </c>
       <c r="F1">
-        <v>3</v>
+        <v>1111</v>
       </c>
       <c r="G1" t="s">
         <v>2</v>
@@ -465,24 +561,93 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D2">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="E2">
+        <v>112</v>
+      </c>
+      <c r="F2">
+        <v>1112</v>
+      </c>
+      <c r="G2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3">
         <v>3</v>
       </c>
-      <c r="F2">
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3">
+        <v>13</v>
+      </c>
+      <c r="E3">
+        <v>113</v>
+      </c>
+      <c r="F3">
+        <v>1113</v>
+      </c>
+      <c r="G3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4">
         <v>4</v>
       </c>
-      <c r="G2" t="s">
-        <v>4</v>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4">
+        <v>14</v>
+      </c>
+      <c r="E4">
+        <v>114</v>
+      </c>
+      <c r="F4">
+        <v>1114</v>
+      </c>
+      <c r="G4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5">
+        <v>15</v>
+      </c>
+      <c r="E5">
+        <v>115</v>
+      </c>
+      <c r="F5">
+        <v>1115</v>
+      </c>
+      <c r="G5" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
ROBE-139 Enum type parsers
</commit_message>
<xml_diff>
--- a/robe-convert/src/test/resources/sample.xlsx
+++ b/robe-convert/src/test/resources/sample.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
   <si>
     <t>Seray</t>
   </si>
@@ -64,6 +64,12 @@
   </si>
   <si>
     <t>05.01.2014</t>
+  </si>
+  <si>
+    <t>SAMPLE1</t>
+  </si>
+  <si>
+    <t>SAMPLE2</t>
   </si>
 </sst>
 </file>
@@ -105,8 +111,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -115,11 +123,13 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -517,10 +527,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -530,7 +540,7 @@
     <col min="7" max="7" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8">
       <c r="A1">
         <v>1</v>
       </c>
@@ -552,8 +562,11 @@
       <c r="G1" t="s">
         <v>2</v>
       </c>
+      <c r="H1" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:8">
       <c r="A2">
         <v>2</v>
       </c>
@@ -575,8 +588,11 @@
       <c r="G2" t="s">
         <v>5</v>
       </c>
+      <c r="H2" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:8">
       <c r="A3">
         <v>3</v>
       </c>
@@ -598,8 +614,11 @@
       <c r="G3" t="s">
         <v>8</v>
       </c>
+      <c r="H3" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:8">
       <c r="A4">
         <v>4</v>
       </c>
@@ -621,8 +640,11 @@
       <c r="G4" t="s">
         <v>11</v>
       </c>
+      <c r="H4" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:8">
       <c r="A5">
         <v>5</v>
       </c>
@@ -643,6 +665,9 @@
       </c>
       <c r="G5" t="s">
         <v>14</v>
+      </c>
+      <c r="H5" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ROBE-186 import error for big decimal numbers  larger than 11 digits
</commit_message>
<xml_diff>
--- a/robe-convert/src/test/resources/sample.xlsx
+++ b/robe-convert/src/test/resources/sample.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-23140" yWindow="-20160" windowWidth="14940" windowHeight="12920"/>
+    <workbookView xWindow="-20060" yWindow="-18060" windowWidth="14940" windowHeight="12920"/>
   </bookViews>
   <sheets>
     <sheet name="SamplePojo" sheetId="1" r:id="rId1"/>
@@ -530,13 +530,14 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="F1" sqref="F1:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
     <col min="2" max="2" width="10" customWidth="1"/>
+    <col min="6" max="6" width="14.33203125" customWidth="1"/>
     <col min="7" max="7" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -557,7 +558,7 @@
         <v>111</v>
       </c>
       <c r="F1">
-        <v>1111</v>
+        <v>11111111111</v>
       </c>
       <c r="G1" t="s">
         <v>2</v>
@@ -583,7 +584,7 @@
         <v>112</v>
       </c>
       <c r="F2">
-        <v>1112</v>
+        <v>11111111112</v>
       </c>
       <c r="G2" t="s">
         <v>5</v>
@@ -609,7 +610,7 @@
         <v>113</v>
       </c>
       <c r="F3">
-        <v>1113</v>
+        <v>11111111113</v>
       </c>
       <c r="G3" t="s">
         <v>8</v>
@@ -635,7 +636,7 @@
         <v>114</v>
       </c>
       <c r="F4">
-        <v>1114</v>
+        <v>11111111114</v>
       </c>
       <c r="G4" t="s">
         <v>11</v>
@@ -661,7 +662,7 @@
         <v>115</v>
       </c>
       <c r="F5">
-        <v>1115</v>
+        <v>11111111115</v>
       </c>
       <c r="G5" t="s">
         <v>14</v>
@@ -672,7 +673,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>